<commit_message>
script cleaning - data description
</commit_message>
<xml_diff>
--- a/data/raw-data/2024.10.30_12SV5_eDNA_abundance_samplecorrected.xlsx
+++ b/data/raw-data/2024.10.30_12SV5_eDNA_abundance_samplecorrected.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aloïsito\Documents\Nextcloud\MyDrive\teletravail mercredi 29102024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berardal\Documents\Aloïs\BePrep\00_Papier_substrats\raw_data (pour diffusion)\data_used_for_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDAA947-3C12-4F89-8FD0-5407E49199C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Merge_taxa (2)" sheetId="6" r:id="rId1"/>
@@ -2848,7 +2847,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3703,15 +3702,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:NZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="20" ySplit="1" topLeftCell="LH31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="20" ySplit="1" topLeftCell="LH28" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="LT2" sqref="LS2:LT69"/>
+      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -48288,7 +48287,7 @@
         <v>59</v>
       </c>
       <c r="K39" t="s">
-        <v>59</v>
+        <v>485</v>
       </c>
       <c r="M39" t="s">
         <v>72</v>
@@ -84496,8 +84495,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:NZ1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:OL69">
+  <autoFilter ref="A1:NZ1">
+    <sortState ref="A2:OL69">
       <sortCondition ref="T1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added repeat model that fits using binomial
</commit_message>
<xml_diff>
--- a/data/raw-data/2024.10.30_12SV5_eDNA_abundance_samplecorrected.xlsx
+++ b/data/raw-data/2024.10.30_12SV5_eDNA_abundance_samplecorrected.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="939">
   <si>
     <t>#comment</t>
   </si>
@@ -2248,9 +2248,6 @@
   </si>
   <si>
     <t>Tyrannidae</t>
-  </si>
-  <si>
-    <t>Tyrannus</t>
   </si>
   <si>
     <t>1.44e-41</t>
@@ -3706,11 +3703,11 @@
   <dimension ref="A1:NZ69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="20" ySplit="1" topLeftCell="LH28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="20" ySplit="1" topLeftCell="V10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3862,10 +3859,10 @@
         <v>60</v>
       </c>
       <c r="K1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="L1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M1" t="s">
         <v>70</v>
@@ -4372,13 +4369,13 @@
         <v>278</v>
       </c>
       <c r="FY1" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="FZ1" s="2" t="s">
         <v>932</v>
       </c>
-      <c r="FZ1" s="2" t="s">
+      <c r="GA1" s="2" t="s">
         <v>933</v>
-      </c>
-      <c r="GA1" s="2" t="s">
-        <v>934</v>
       </c>
       <c r="GB1" s="2" t="s">
         <v>279</v>
@@ -4678,13 +4675,13 @@
         <v>377</v>
       </c>
       <c r="JW1" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="JX1" s="2" t="s">
         <v>929</v>
       </c>
-      <c r="JX1" s="2" t="s">
+      <c r="JY1" s="2" t="s">
         <v>930</v>
-      </c>
-      <c r="JY1" s="2" t="s">
-        <v>931</v>
       </c>
       <c r="JZ1" s="2" t="s">
         <v>378</v>
@@ -4732,16 +4729,16 @@
         <v>392</v>
       </c>
       <c r="KO1" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="KP1" s="2" t="s">
         <v>926</v>
       </c>
-      <c r="KP1" s="2" t="s">
+      <c r="KQ1" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="KQ1" s="2" t="s">
-        <v>928</v>
-      </c>
       <c r="KR1" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="KS1" s="2" t="s">
         <v>393</v>
@@ -4786,13 +4783,13 @@
         <v>406</v>
       </c>
       <c r="LG1" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="LH1" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="LH1" s="2" t="s">
+      <c r="LI1" s="2" t="s">
         <v>921</v>
-      </c>
-      <c r="LI1" s="2" t="s">
-        <v>922</v>
       </c>
       <c r="LJ1" s="2" t="s">
         <v>407</v>
@@ -4804,28 +4801,28 @@
         <v>409</v>
       </c>
       <c r="LM1" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="LN1" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="LO1" s="2" t="s">
         <v>410</v>
       </c>
       <c r="LP1" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="LQ1" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="LQ1" s="2" t="s">
+      <c r="LR1" s="2" t="s">
         <v>924</v>
       </c>
-      <c r="LR1" s="2" t="s">
-        <v>925</v>
-      </c>
       <c r="LS1" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="LT1" s="2" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="LU1" s="2" t="s">
         <v>411</v>
@@ -4840,13 +4837,13 @@
         <v>414</v>
       </c>
       <c r="LY1" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="LZ1" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="LZ1" s="2" t="s">
+      <c r="MA1" s="2" t="s">
         <v>918</v>
-      </c>
-      <c r="MA1" s="2" t="s">
-        <v>919</v>
       </c>
       <c r="MB1" s="2" t="s">
         <v>415</v>
@@ -4903,13 +4900,13 @@
         <v>432</v>
       </c>
       <c r="MT1" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="MU1" s="2" t="s">
         <v>914</v>
       </c>
-      <c r="MU1" s="2" t="s">
+      <c r="MV1" s="2" t="s">
         <v>915</v>
-      </c>
-      <c r="MV1" s="2" t="s">
-        <v>916</v>
       </c>
       <c r="MW1" s="2" t="s">
         <v>433</v>
@@ -6200,10 +6197,10 @@
         <v>52</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M3" t="s">
         <v>72</v>
@@ -7345,10 +7342,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>808</v>
+      </c>
+      <c r="C4" t="s">
         <v>809</v>
-      </c>
-      <c r="C4" t="s">
-        <v>810</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -7360,19 +7357,19 @@
         <v>31</v>
       </c>
       <c r="G4" t="s">
+        <v>801</v>
+      </c>
+      <c r="H4" t="s">
         <v>802</v>
       </c>
-      <c r="H4" t="s">
-        <v>803</v>
-      </c>
       <c r="I4" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="M4" t="s">
         <v>72</v>
@@ -7384,19 +7381,19 @@
         <v>74</v>
       </c>
       <c r="P4" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="Q4">
         <v>100</v>
       </c>
       <c r="R4" t="s">
+        <v>812</v>
+      </c>
+      <c r="S4" t="s">
         <v>813</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>814</v>
-      </c>
-      <c r="T4" t="s">
-        <v>815</v>
       </c>
       <c r="U4">
         <v>5</v>
@@ -8535,13 +8532,13 @@
         <v>570</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="M5" t="s">
         <v>72</v>
@@ -9683,7 +9680,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -9698,19 +9695,19 @@
         <v>31</v>
       </c>
       <c r="G6" t="s">
+        <v>846</v>
+      </c>
+      <c r="H6" t="s">
         <v>847</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>848</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>849</v>
       </c>
-      <c r="J6" t="s">
-        <v>850</v>
-      </c>
       <c r="K6" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="M6" t="s">
         <v>72</v>
@@ -9728,13 +9725,13 @@
         <v>99</v>
       </c>
       <c r="R6" t="s">
+        <v>850</v>
+      </c>
+      <c r="S6" t="s">
         <v>851</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>852</v>
-      </c>
-      <c r="T6" t="s">
-        <v>853</v>
       </c>
       <c r="U6">
         <v>17901</v>
@@ -10873,13 +10870,13 @@
         <v>570</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J7" t="s">
         <v>59</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="M7" t="s">
         <v>72</v>
@@ -12021,10 +12018,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>773</v>
+      </c>
+      <c r="C8" t="s">
         <v>774</v>
-      </c>
-      <c r="C8" t="s">
-        <v>775</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -12033,22 +12030,22 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
+        <v>775</v>
+      </c>
+      <c r="G8" t="s">
         <v>776</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>777</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>778</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>779</v>
       </c>
-      <c r="J8" t="s">
-        <v>780</v>
-      </c>
       <c r="K8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="M8" t="s">
         <v>72</v>
@@ -12066,13 +12063,13 @@
         <v>100</v>
       </c>
       <c r="R8" t="s">
+        <v>780</v>
+      </c>
+      <c r="S8" t="s">
         <v>781</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>782</v>
-      </c>
-      <c r="T8" t="s">
-        <v>783</v>
       </c>
       <c r="U8">
         <v>343</v>
@@ -14379,14 +14376,14 @@
       <c r="H10" t="s">
         <v>741</v>
       </c>
-      <c r="I10" t="s">
-        <v>742</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K10" t="s">
-        <v>742</v>
+      <c r="J10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>741</v>
       </c>
       <c r="M10" t="s">
         <v>72</v>
@@ -14398,19 +14395,19 @@
         <v>74</v>
       </c>
       <c r="P10" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Q10">
         <v>101</v>
       </c>
       <c r="R10" t="s">
+        <v>743</v>
+      </c>
+      <c r="S10" t="s">
         <v>744</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>745</v>
-      </c>
-      <c r="T10" t="s">
-        <v>746</v>
       </c>
       <c r="U10">
         <v>263</v>
@@ -15552,10 +15549,10 @@
         <v>615</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="M11" t="s">
         <v>72</v>
@@ -20225,13 +20222,13 @@
         <v>698</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J15" t="s">
         <v>59</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="M15" t="s">
         <v>72</v>
@@ -21400,7 +21397,7 @@
         <v>59</v>
       </c>
       <c r="K16" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="M16" t="s">
         <v>72</v>
@@ -24880,10 +24877,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>763</v>
+      </c>
+      <c r="C19" t="s">
         <v>764</v>
-      </c>
-      <c r="C19" t="s">
-        <v>765</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -24895,43 +24892,43 @@
         <v>507</v>
       </c>
       <c r="G19" t="s">
+        <v>757</v>
+      </c>
+      <c r="H19" t="s">
         <v>758</v>
       </c>
-      <c r="H19" t="s">
-        <v>759</v>
-      </c>
       <c r="I19" t="s">
+        <v>765</v>
+      </c>
+      <c r="J19" t="s">
         <v>766</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
+        <v>766</v>
+      </c>
+      <c r="M19" t="s">
         <v>767</v>
       </c>
-      <c r="K19" t="s">
-        <v>767</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>768</v>
-      </c>
-      <c r="N19" t="s">
-        <v>769</v>
       </c>
       <c r="O19" t="s">
         <v>74</v>
       </c>
       <c r="P19" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="Q19">
         <v>106</v>
       </c>
       <c r="R19" t="s">
+        <v>770</v>
+      </c>
+      <c r="S19" t="s">
         <v>771</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>772</v>
-      </c>
-      <c r="T19" t="s">
-        <v>773</v>
       </c>
       <c r="U19">
         <v>11956</v>
@@ -28387,10 +28384,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>860</v>
+      </c>
+      <c r="C22" t="s">
         <v>861</v>
-      </c>
-      <c r="C22" t="s">
-        <v>862</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -28402,19 +28399,19 @@
         <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H22" t="s">
+        <v>862</v>
+      </c>
+      <c r="I22" t="s">
         <v>863</v>
-      </c>
-      <c r="I22" t="s">
-        <v>864</v>
       </c>
       <c r="J22" t="s">
         <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="M22" t="s">
         <v>72</v>
@@ -28432,13 +28429,13 @@
         <v>101</v>
       </c>
       <c r="R22" t="s">
+        <v>864</v>
+      </c>
+      <c r="S22" t="s">
         <v>865</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>866</v>
-      </c>
-      <c r="T22" t="s">
-        <v>867</v>
       </c>
       <c r="U22">
         <v>104</v>
@@ -33063,10 +33060,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>822</v>
+      </c>
+      <c r="C26" t="s">
         <v>823</v>
-      </c>
-      <c r="C26" t="s">
-        <v>824</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
@@ -33078,19 +33075,19 @@
         <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H26" t="s">
+        <v>824</v>
+      </c>
+      <c r="I26" t="s">
         <v>825</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>826</v>
       </c>
-      <c r="J26" t="s">
-        <v>827</v>
-      </c>
       <c r="K26" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="M26" t="s">
         <v>72</v>
@@ -33108,13 +33105,13 @@
         <v>100</v>
       </c>
       <c r="R26" t="s">
+        <v>827</v>
+      </c>
+      <c r="S26" t="s">
         <v>828</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>829</v>
-      </c>
-      <c r="T26" t="s">
-        <v>830</v>
       </c>
       <c r="U26">
         <v>6761</v>
@@ -34232,10 +34229,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>815</v>
+      </c>
+      <c r="C27" t="s">
         <v>816</v>
-      </c>
-      <c r="C27" t="s">
-        <v>817</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
@@ -34247,19 +34244,19 @@
         <v>31</v>
       </c>
       <c r="G27" t="s">
+        <v>801</v>
+      </c>
+      <c r="H27" t="s">
         <v>802</v>
       </c>
-      <c r="H27" t="s">
-        <v>803</v>
-      </c>
       <c r="I27" t="s">
+        <v>817</v>
+      </c>
+      <c r="J27" t="s">
         <v>818</v>
       </c>
-      <c r="J27" t="s">
-        <v>819</v>
-      </c>
       <c r="K27" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="M27" t="s">
         <v>72</v>
@@ -34277,13 +34274,13 @@
         <v>100</v>
       </c>
       <c r="R27" t="s">
+        <v>819</v>
+      </c>
+      <c r="S27" t="s">
         <v>820</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>821</v>
-      </c>
-      <c r="T27" t="s">
-        <v>822</v>
       </c>
       <c r="U27">
         <v>9608</v>
@@ -36570,10 +36567,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>867</v>
+      </c>
+      <c r="C29" t="s">
         <v>868</v>
-      </c>
-      <c r="C29" t="s">
-        <v>869</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
@@ -36585,19 +36582,19 @@
         <v>31</v>
       </c>
       <c r="G29" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H29" t="s">
+        <v>869</v>
+      </c>
+      <c r="I29" t="s">
         <v>870</v>
       </c>
-      <c r="I29" t="s">
-        <v>871</v>
-      </c>
       <c r="J29" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="M29" t="s">
         <v>72</v>
@@ -36615,13 +36612,13 @@
         <v>100</v>
       </c>
       <c r="R29" t="s">
+        <v>871</v>
+      </c>
+      <c r="S29" t="s">
         <v>872</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>873</v>
-      </c>
-      <c r="T29" t="s">
-        <v>874</v>
       </c>
       <c r="U29">
         <v>43</v>
@@ -43605,16 +43602,16 @@
         <v>501</v>
       </c>
       <c r="I35" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="M35" s="4" t="s">
         <v>883</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>882</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>882</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>884</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>74</v>
@@ -43623,7 +43620,7 @@
         <v>74</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="Q35">
         <v>80</v>
@@ -44777,10 +44774,10 @@
         <v>628</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="M36" t="s">
         <v>72</v>
@@ -45922,10 +45919,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>783</v>
+      </c>
+      <c r="C37" t="s">
         <v>784</v>
-      </c>
-      <c r="C37" t="s">
-        <v>785</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -45934,25 +45931,25 @@
         <v>29</v>
       </c>
       <c r="F37" t="s">
+        <v>775</v>
+      </c>
+      <c r="G37" t="s">
         <v>776</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>777</v>
       </c>
-      <c r="H37" t="s">
-        <v>778</v>
-      </c>
       <c r="I37" t="s">
+        <v>785</v>
+      </c>
+      <c r="J37" t="s">
         <v>786</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
+        <v>786</v>
+      </c>
+      <c r="M37" t="s">
         <v>787</v>
-      </c>
-      <c r="K37" t="s">
-        <v>787</v>
-      </c>
-      <c r="M37" t="s">
-        <v>788</v>
       </c>
       <c r="N37" t="s">
         <v>74</v>
@@ -45967,13 +45964,13 @@
         <v>101</v>
       </c>
       <c r="R37" t="s">
+        <v>788</v>
+      </c>
+      <c r="S37" t="s">
         <v>789</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>790</v>
-      </c>
-      <c r="T37" t="s">
-        <v>791</v>
       </c>
       <c r="U37">
         <v>3103</v>
@@ -50622,10 +50619,10 @@
         <v>555</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="M41" t="s">
         <v>72</v>
@@ -51767,10 +51764,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>799</v>
+      </c>
+      <c r="C42" t="s">
         <v>800</v>
-      </c>
-      <c r="C42" t="s">
-        <v>801</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -51782,19 +51779,19 @@
         <v>31</v>
       </c>
       <c r="G42" t="s">
+        <v>801</v>
+      </c>
+      <c r="H42" t="s">
         <v>802</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>803</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>804</v>
       </c>
-      <c r="J42" t="s">
-        <v>805</v>
-      </c>
       <c r="K42" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="M42" t="s">
         <v>72</v>
@@ -51812,13 +51809,13 @@
         <v>100</v>
       </c>
       <c r="R42" t="s">
+        <v>805</v>
+      </c>
+      <c r="S42" t="s">
         <v>806</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>807</v>
-      </c>
-      <c r="T42" t="s">
-        <v>808</v>
       </c>
       <c r="U42">
         <v>38929</v>
@@ -55295,13 +55292,13 @@
         <v>711</v>
       </c>
       <c r="I45" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>898</v>
       </c>
-      <c r="J45" s="4" t="s">
-        <v>899</v>
-      </c>
       <c r="K45" s="4" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="M45" t="s">
         <v>72</v>
@@ -56470,7 +56467,7 @@
         <v>59</v>
       </c>
       <c r="K46" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="M46" t="s">
         <v>72</v>
@@ -57633,13 +57630,13 @@
         <v>570</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="M47" t="s">
         <v>72</v>
@@ -58781,10 +58778,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
+        <v>853</v>
+      </c>
+      <c r="C48" t="s">
         <v>854</v>
-      </c>
-      <c r="C48" t="s">
-        <v>855</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -58796,19 +58793,19 @@
         <v>31</v>
       </c>
       <c r="G48" t="s">
+        <v>846</v>
+      </c>
+      <c r="H48" t="s">
         <v>847</v>
       </c>
-      <c r="H48" t="s">
-        <v>848</v>
-      </c>
       <c r="I48" t="s">
+        <v>855</v>
+      </c>
+      <c r="J48" t="s">
         <v>856</v>
       </c>
-      <c r="J48" t="s">
-        <v>857</v>
-      </c>
       <c r="K48" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="M48" t="s">
         <v>72</v>
@@ -58826,13 +58823,13 @@
         <v>99</v>
       </c>
       <c r="R48" t="s">
+        <v>857</v>
+      </c>
+      <c r="S48" t="s">
         <v>858</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>859</v>
-      </c>
-      <c r="T48" t="s">
-        <v>860</v>
       </c>
       <c r="U48">
         <v>1477</v>
@@ -59968,7 +59965,7 @@
         <v>613</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I49" t="s">
         <v>59</v>
@@ -59977,7 +59974,7 @@
         <v>59</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="M49" t="s">
         <v>72</v>
@@ -61119,10 +61116,10 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>755</v>
+      </c>
+      <c r="C50" t="s">
         <v>756</v>
-      </c>
-      <c r="C50" t="s">
-        <v>757</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -61134,19 +61131,19 @@
         <v>507</v>
       </c>
       <c r="G50" t="s">
+        <v>757</v>
+      </c>
+      <c r="H50" t="s">
         <v>758</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>759</v>
       </c>
-      <c r="I50" t="s">
-        <v>760</v>
-      </c>
       <c r="J50" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="M50" t="s">
         <v>72</v>
@@ -61164,13 +61161,13 @@
         <v>101</v>
       </c>
       <c r="R50" t="s">
+        <v>760</v>
+      </c>
+      <c r="S50" t="s">
         <v>761</v>
       </c>
-      <c r="S50" t="s">
+      <c r="T50" t="s">
         <v>762</v>
-      </c>
-      <c r="T50" t="s">
-        <v>763</v>
       </c>
       <c r="U50">
         <v>2074</v>
@@ -62288,10 +62285,10 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>830</v>
+      </c>
+      <c r="C51" t="s">
         <v>831</v>
-      </c>
-      <c r="C51" t="s">
-        <v>832</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
@@ -62303,19 +62300,19 @@
         <v>31</v>
       </c>
       <c r="G51" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H51" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="I51" t="s">
+        <v>832</v>
+      </c>
+      <c r="J51" t="s">
         <v>833</v>
       </c>
-      <c r="J51" t="s">
-        <v>834</v>
-      </c>
       <c r="K51" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M51" t="s">
         <v>72</v>
@@ -62333,13 +62330,13 @@
         <v>100</v>
       </c>
       <c r="R51" t="s">
+        <v>834</v>
+      </c>
+      <c r="S51" t="s">
         <v>835</v>
       </c>
-      <c r="S51" t="s">
+      <c r="T51" t="s">
         <v>836</v>
-      </c>
-      <c r="T51" t="s">
-        <v>837</v>
       </c>
       <c r="U51">
         <v>1309</v>
@@ -64626,10 +64623,10 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>837</v>
+      </c>
+      <c r="C53" t="s">
         <v>838</v>
-      </c>
-      <c r="C53" t="s">
-        <v>839</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
@@ -64641,19 +64638,19 @@
         <v>31</v>
       </c>
       <c r="G53" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H53" t="s">
+        <v>839</v>
+      </c>
+      <c r="I53" t="s">
         <v>840</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>841</v>
       </c>
-      <c r="J53" t="s">
-        <v>842</v>
-      </c>
       <c r="K53" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="M53" t="s">
         <v>72</v>
@@ -64671,13 +64668,13 @@
         <v>99</v>
       </c>
       <c r="R53" t="s">
+        <v>842</v>
+      </c>
+      <c r="S53" t="s">
         <v>843</v>
       </c>
-      <c r="S53" t="s">
+      <c r="T53" t="s">
         <v>844</v>
-      </c>
-      <c r="T53" t="s">
-        <v>845</v>
       </c>
       <c r="U53">
         <v>20651</v>
@@ -65816,13 +65813,13 @@
         <v>570</v>
       </c>
       <c r="I54" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>888</v>
       </c>
-      <c r="J54" s="4" t="s">
-        <v>889</v>
-      </c>
       <c r="K54" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="M54" t="s">
         <v>72</v>
@@ -68157,10 +68154,10 @@
         <v>705</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="M56" t="s">
         <v>72</v>
@@ -70471,10 +70468,10 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
+        <v>791</v>
+      </c>
+      <c r="C58" t="s">
         <v>792</v>
-      </c>
-      <c r="C58" t="s">
-        <v>793</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
@@ -70483,22 +70480,22 @@
         <v>29</v>
       </c>
       <c r="F58" t="s">
+        <v>775</v>
+      </c>
+      <c r="G58" t="s">
         <v>776</v>
       </c>
-      <c r="G58" t="s">
-        <v>777</v>
-      </c>
       <c r="H58" t="s">
+        <v>793</v>
+      </c>
+      <c r="I58" t="s">
         <v>794</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>795</v>
       </c>
-      <c r="J58" t="s">
-        <v>796</v>
-      </c>
       <c r="K58" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="M58" t="s">
         <v>72</v>
@@ -70516,13 +70513,13 @@
         <v>97</v>
       </c>
       <c r="R58" t="s">
+        <v>796</v>
+      </c>
+      <c r="S58" t="s">
         <v>797</v>
       </c>
-      <c r="S58" t="s">
+      <c r="T58" t="s">
         <v>798</v>
-      </c>
-      <c r="T58" t="s">
-        <v>799</v>
       </c>
       <c r="U58">
         <v>5</v>
@@ -71667,7 +71664,7 @@
         <v>59</v>
       </c>
       <c r="K59" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="M59" t="s">
         <v>72</v>
@@ -73996,16 +73993,16 @@
         <v>613</v>
       </c>
       <c r="H61" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>895</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>896</v>
       </c>
       <c r="J61" t="s">
         <v>59</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="M61" t="s">
         <v>72</v>
@@ -75147,10 +75144,10 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>746</v>
+      </c>
+      <c r="C62" t="s">
         <v>747</v>
-      </c>
-      <c r="C62" t="s">
-        <v>748</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
@@ -75162,19 +75159,19 @@
         <v>507</v>
       </c>
       <c r="G62" t="s">
+        <v>748</v>
+      </c>
+      <c r="H62" t="s">
         <v>749</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>750</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>751</v>
       </c>
-      <c r="J62" t="s">
-        <v>752</v>
-      </c>
       <c r="K62" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="M62" t="s">
         <v>72</v>
@@ -75192,13 +75189,13 @@
         <v>101</v>
       </c>
       <c r="R62" t="s">
+        <v>752</v>
+      </c>
+      <c r="S62" t="s">
         <v>753</v>
       </c>
-      <c r="S62" t="s">
+      <c r="T62" t="s">
         <v>754</v>
-      </c>
-      <c r="T62" t="s">
-        <v>755</v>
       </c>
       <c r="U62">
         <v>1008</v>
@@ -78654,10 +78651,10 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
+        <v>876</v>
+      </c>
+      <c r="C65" t="s">
         <v>877</v>
-      </c>
-      <c r="C65" t="s">
-        <v>878</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
@@ -78669,19 +78666,19 @@
         <v>31</v>
       </c>
       <c r="G65" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H65" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I65" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="J65" s="4" t="s">
         <v>875</v>
       </c>
-      <c r="J65" s="4" t="s">
-        <v>876</v>
-      </c>
       <c r="K65" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="M65" t="s">
         <v>72</v>
@@ -78699,13 +78696,13 @@
         <v>100</v>
       </c>
       <c r="R65" t="s">
+        <v>878</v>
+      </c>
+      <c r="S65" t="s">
         <v>879</v>
       </c>
-      <c r="S65" t="s">
+      <c r="T65" t="s">
         <v>880</v>
-      </c>
-      <c r="T65" t="s">
-        <v>881</v>
       </c>
       <c r="U65">
         <v>1295</v>
@@ -79847,10 +79844,10 @@
         <v>525</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="M66" t="s">
         <v>72</v>
@@ -83354,10 +83351,10 @@
         <v>494</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="M69" t="s">
         <v>72</v>

</xml_diff>